<commit_message>
updated server and ngram writer
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\10-DataScienceCapStone\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="10515" windowHeight="9270"/>
   </bookViews>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="54">
   <si>
     <t>Backlog item</t>
   </si>
@@ -185,16 +180,13 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,9 +244,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -292,9 +284,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,10 +318,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -361,10 +352,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -537,14 +527,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
@@ -553,13 +543,13 @@
     <col min="6" max="6" width="93.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="42.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -582,7 +572,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -596,7 +586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="18" customHeight="1">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -613,7 +603,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -630,7 +620,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="45">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -647,7 +637,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -661,10 +651,10 @@
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -678,10 +668,10 @@
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -698,7 +688,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -715,7 +705,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -732,7 +722,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -749,7 +739,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -766,7 +756,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="4">
         <v>2</v>
       </c>
@@ -777,12 +767,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="4">
         <v>2</v>
       </c>
@@ -793,12 +783,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="4">
         <v>2</v>
       </c>
@@ -809,12 +799,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="4">
         <v>2</v>
       </c>
@@ -825,7 +815,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -842,7 +832,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>3</v>
       </c>
@@ -853,12 +843,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>3</v>
       </c>
@@ -869,12 +859,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>3</v>
       </c>
@@ -885,7 +875,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -902,7 +892,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>4</v>
       </c>
@@ -913,12 +903,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>4</v>
       </c>
@@ -929,12 +919,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>4</v>
       </c>
@@ -945,7 +935,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -962,7 +952,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>5</v>
       </c>
@@ -973,12 +963,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>5</v>
       </c>
@@ -989,7 +979,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -1006,7 +996,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>6</v>
       </c>
@@ -1017,12 +1007,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>6</v>
       </c>
@@ -1033,7 +1023,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -1057,14 +1047,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
@@ -1073,13 +1063,13 @@
     <col min="6" max="6" width="93.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="42.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1099,7 +1089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1113,7 +1103,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="18" customHeight="1">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -1127,7 +1117,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -1141,7 +1131,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="45">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -1155,7 +1145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -1169,7 +1159,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="4"/>
       <c r="B8" s="2">
         <v>42462</v>
@@ -1181,7 +1171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -1195,7 +1185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -1209,7 +1199,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -1223,7 +1213,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -1237,7 +1227,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="4">
         <v>1</v>
       </c>
@@ -1251,7 +1241,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1268,7 +1258,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="4">
         <v>2</v>
       </c>
@@ -1279,12 +1269,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="4">
         <v>2</v>
       </c>
@@ -1295,12 +1285,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="4">
         <v>2</v>
       </c>
@@ -1311,12 +1301,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="4">
         <v>2</v>
       </c>
@@ -1327,7 +1317,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1344,7 +1334,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1355,12 +1345,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1371,12 +1361,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1387,7 +1377,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1404,7 +1394,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1415,12 +1405,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1431,12 +1421,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1447,7 +1437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1464,7 +1454,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>5</v>
       </c>
@@ -1475,12 +1465,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>5</v>
       </c>
@@ -1491,7 +1481,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -1508,7 +1498,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>6</v>
       </c>
@@ -1519,12 +1509,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>6</v>
       </c>
@@ -1535,7 +1525,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
update with inital test
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\10-DataScienceCapStone\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="10515" windowHeight="9270"/>
   </bookViews>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="71">
   <si>
     <t>Backlog item</t>
   </si>
@@ -241,8 +236,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,9 +295,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -340,9 +335,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -374,10 +369,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -409,10 +403,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -585,14 +578,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
@@ -601,13 +594,13 @@
     <col min="6" max="6" width="93.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="42.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -630,7 +623,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -644,7 +637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="18" customHeight="1">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -661,7 +654,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -678,7 +671,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="45">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -695,7 +688,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -712,7 +705,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -729,7 +722,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -746,7 +739,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -763,7 +756,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -780,7 +773,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -797,7 +790,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="4">
         <v>1</v>
       </c>
@@ -811,10 +804,10 @@
         <v>65</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -831,7 +824,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
         <v>70</v>
       </c>
@@ -842,7 +835,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="4"/>
       <c r="E16">
         <v>1</v>
@@ -851,7 +844,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="4">
         <v>2</v>
       </c>
@@ -862,7 +855,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="4"/>
       <c r="E18">
         <v>3</v>
@@ -871,298 +864,307 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>2</v>
-      </c>
-      <c r="C19" s="3" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" s="4"/>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="4">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="4"/>
       <c r="E21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="4"/>
       <c r="E22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="4"/>
       <c r="E23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="4"/>
       <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="4"/>
+      <c r="E25">
         <v>5</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>2</v>
-      </c>
-      <c r="E25">
+    <row r="26" spans="1:6">
+      <c r="A26" s="4">
+        <v>2</v>
+      </c>
+      <c r="E26">
         <v>6</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>2</v>
-      </c>
-      <c r="C26" s="3" t="s">
+    <row r="27" spans="1:6">
+      <c r="A27" s="4">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27" t="s">
+    <row r="28" spans="1:6">
+      <c r="A28" s="4"/>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>2</v>
-      </c>
-      <c r="C29" s="3" t="s">
+    <row r="29" spans="1:6">
+      <c r="A29" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:6">
+      <c r="A31" s="4"/>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>3</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>2</v>
-      </c>
-      <c r="C35" s="3" t="s">
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="4">
+        <v>2</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>4</v>
       </c>
-      <c r="C38" s="3" t="s">
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="41" spans="1:6">
+      <c r="A41">
         <v>3</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>4</v>
       </c>
-      <c r="C42" s="3" t="s">
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>5</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46">
-        <v>6</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C47" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>6</v>
       </c>
-      <c r="C48" s="3" t="s">
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <v>6</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F49" s="5" t="s">
+      <c r="B50" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1173,14 +1175,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
@@ -1189,13 +1191,13 @@
     <col min="6" max="6" width="93.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="42.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1215,7 +1217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1229,7 +1231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="18" customHeight="1">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -1243,7 +1245,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -1257,7 +1259,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="45">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -1271,7 +1273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -1285,7 +1287,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="4"/>
       <c r="B8" s="2">
         <v>42462</v>
@@ -1297,7 +1299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -1311,7 +1313,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -1325,7 +1327,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -1339,7 +1341,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -1353,7 +1355,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="4">
         <v>1</v>
       </c>
@@ -1367,7 +1369,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1384,7 +1386,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="4">
         <v>2</v>
       </c>
@@ -1395,12 +1397,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="4">
         <v>2</v>
       </c>
@@ -1411,12 +1413,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="4">
         <v>2</v>
       </c>
@@ -1427,12 +1429,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="4">
         <v>2</v>
       </c>
@@ -1443,7 +1445,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1460,7 +1462,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1471,12 +1473,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1487,12 +1489,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1503,7 +1505,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1520,7 +1522,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1531,12 +1533,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1547,12 +1549,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1563,7 +1565,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1580,7 +1582,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>5</v>
       </c>
@@ -1591,12 +1593,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>5</v>
       </c>
@@ -1607,7 +1609,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -1624,7 +1626,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>6</v>
       </c>
@@ -1635,12 +1637,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>6</v>
       </c>
@@ -1651,7 +1653,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Implemented faster lookup and kneser ney
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="74">
   <si>
     <t>Backlog item</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Ready</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
@@ -218,9 +215,6 @@
     <t>Deploy to shinyapps</t>
   </si>
   <si>
-    <t>Release 2: 15.4.2016</t>
-  </si>
-  <si>
     <t>Release 3: 17.4.2016</t>
   </si>
   <si>
@@ -231,6 +225,21 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Release 2: 16.4.2016</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>review and consolidate common function</t>
+  </si>
+  <si>
+    <t>Need to extract strings with at least two tokens</t>
+  </si>
+  <si>
+    <t>Improve memory usage and response time</t>
   </si>
 </sst>
 </file>
@@ -579,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -651,7 +660,7 @@
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -668,7 +677,7 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45">
@@ -685,7 +694,7 @@
         <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -702,7 +711,7 @@
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -719,7 +728,7 @@
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -736,7 +745,7 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -753,7 +762,7 @@
         <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -770,7 +779,7 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -801,15 +810,15 @@
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>42</v>
@@ -826,7 +835,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>49</v>
@@ -841,39 +850,39 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="4">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:8">
       <c r="A18" s="4"/>
       <c r="E18">
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="4"/>
       <c r="E19">
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="4">
         <v>2</v>
       </c>
@@ -884,52 +893,70 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:8">
       <c r="A21" s="4"/>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>57</v>
+      </c>
+      <c r="G21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="4"/>
       <c r="E22">
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>59</v>
+      </c>
+      <c r="G22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="4"/>
       <c r="E23">
         <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>62</v>
+      </c>
+      <c r="G23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="4"/>
       <c r="E24">
         <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>58</v>
+      </c>
+      <c r="G24" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="4"/>
       <c r="E25">
         <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="G25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="4">
         <v>2</v>
       </c>
@@ -937,10 +964,13 @@
         <v>6</v>
       </c>
       <c r="F26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>61</v>
+      </c>
+      <c r="G26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="4">
         <v>2</v>
       </c>
@@ -951,69 +981,79 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:8">
       <c r="A28" s="4"/>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30">
-        <v>2</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="4"/>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="4"/>
-      <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>42</v>
+    <row r="32" spans="1:8">
+      <c r="A32" s="4"/>
+      <c r="E32">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33">
-        <v>3</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D33" t="s">
-        <v>16</v>
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
         <v>3</v>
       </c>
+      <c r="C34" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
@@ -1021,150 +1061,155 @@
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="4">
-        <v>2</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="A36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="4">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>67</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="38" spans="1:6">
-      <c r="A38">
-        <v>4</v>
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39">
         <v>4</v>
       </c>
-      <c r="C39" s="3" t="s">
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D39" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41">
-        <v>3</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D41" t="s">
-        <v>24</v>
+      <c r="D40" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43">
         <v>4</v>
       </c>
-      <c r="C43" s="3" t="s">
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="45" spans="1:6">
-      <c r="A45">
-        <v>5</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" t="s">
-        <v>19</v>
+      <c r="A45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46">
         <v>5</v>
       </c>
+      <c r="C46" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47">
-        <v>6</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D47" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48">
         <v>6</v>
       </c>
+      <c r="C48" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49">
         <v>6</v>
       </c>
-      <c r="C49" s="3" t="s">
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>6</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" t="s">
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F50" s="5" t="s">
+      <c r="B51" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated readme, server and ui
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="117">
   <si>
     <t>Backlog item</t>
   </si>
@@ -366,6 +366,9 @@
   </si>
   <si>
     <t>Satureday</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -717,7 +720,7 @@
   <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+      <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1427,21 +1430,33 @@
       <c r="F67" t="s">
         <v>92</v>
       </c>
+      <c r="G67" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="68" spans="2:7">
       <c r="F68" t="s">
         <v>93</v>
       </c>
+      <c r="G68" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="69" spans="2:7">
       <c r="F69" t="s">
         <v>94</v>
       </c>
+      <c r="G69" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="70" spans="2:7">
       <c r="F70" t="s">
         <v>95</v>
       </c>
+      <c r="G70" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="72" spans="2:7">
       <c r="C72" s="3" t="s">
@@ -1455,11 +1470,17 @@
       <c r="F73" t="s">
         <v>102</v>
       </c>
+      <c r="G73" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="74" spans="2:7">
       <c r="F74" t="s">
         <v>103</v>
       </c>
+      <c r="G74" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="75" spans="2:7">
       <c r="C75" s="3" t="s">
@@ -1473,11 +1494,17 @@
       <c r="F76" t="s">
         <v>97</v>
       </c>
+      <c r="G76" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="77" spans="2:7">
       <c r="F77" t="s">
         <v>96</v>
       </c>
+      <c r="G77" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="78" spans="2:7">
       <c r="F78" t="s">
@@ -1494,12 +1521,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:7">
       <c r="F81" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:7">
       <c r="C83" s="3" t="s">
         <v>113</v>
       </c>
@@ -1507,32 +1534,32 @@
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:7">
       <c r="F84" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:7">
       <c r="F85" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:7">
       <c r="F86" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:7">
       <c r="F87" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:7">
       <c r="F88" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:7">
       <c r="C89" s="3" t="s">
         <v>114</v>
       </c>
@@ -1540,12 +1567,15 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:7">
       <c r="F90" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="91" spans="1:6">
+      <c r="G90" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>47</v>
       </c>
@@ -1562,7 +1592,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:7">
       <c r="A93">
         <v>5</v>
       </c>
@@ -1573,7 +1603,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:7">
       <c r="A95">
         <v>4</v>
       </c>

</xml_diff>